<commit_message>
Class 28 Reading data from properties file
</commit_message>
<xml_diff>
--- a/Data/Test.xlsx
+++ b/Data/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/SDETBatch14Java/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352270E6-556B-EC4E-88D1-32B098C95435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFAFE9E-9966-CC4E-AC47-0A76EB3E0495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34020" yWindow="500" windowWidth="34620" windowHeight="22120" xr2:uid="{29CF383E-2365-FC43-AD29-8BB972812F0A}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>